<commit_message>
got it on the SSH
</commit_message>
<xml_diff>
--- a/configs/test_diagnostics.xlsx
+++ b/configs/test_diagnostics.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H128"/>
+  <dimension ref="A1:H134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3796,12 +3796,192 @@
       </c>
       <c r="E128" t="inlineStr"/>
       <c r="F128" s="2" t="n">
-        <v>45912.65889356853</v>
+        <v>45912.65889356482</v>
       </c>
       <c r="G128" s="2" t="n">
-        <v>45912.65889335222</v>
+        <v>45912.65889335648</v>
       </c>
       <c r="H128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr"/>
+      <c r="F129" s="2" t="n">
+        <v>45913.53986631944</v>
+      </c>
+      <c r="G129" s="2" t="n">
+        <v>45913.53986611111</v>
+      </c>
+      <c r="H129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr"/>
+      <c r="F130" s="2" t="n">
+        <v>45913.53986631944</v>
+      </c>
+      <c r="G130" s="2" t="n">
+        <v>45913.53986611111</v>
+      </c>
+      <c r="H130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr"/>
+      <c r="F131" s="2" t="n">
+        <v>45913.61776412037</v>
+      </c>
+      <c r="G131" s="2" t="n">
+        <v>45913.61776390046</v>
+      </c>
+      <c r="H131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr"/>
+      <c r="F132" s="2" t="n">
+        <v>45913.61776412037</v>
+      </c>
+      <c r="G132" s="2" t="n">
+        <v>45913.61776390046</v>
+      </c>
+      <c r="H132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr"/>
+      <c r="F133" s="2" t="n">
+        <v>45913.61797832176</v>
+      </c>
+      <c r="G133" s="2" t="n">
+        <v>45913.61797810185</v>
+      </c>
+      <c r="H133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr"/>
+      <c r="F134" s="2" t="n">
+        <v>45913.61797831874</v>
+      </c>
+      <c r="G134" s="2" t="n">
+        <v>45913.61797810689</v>
+      </c>
+      <c r="H134" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
i have no idea what i changed
</commit_message>
<xml_diff>
--- a/configs/test_diagnostics.xlsx
+++ b/configs/test_diagnostics.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H134"/>
+  <dimension ref="A1:H247"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3976,12 +3976,3402 @@
       </c>
       <c r="E134" t="inlineStr"/>
       <c r="F134" s="2" t="n">
-        <v>45913.61797831874</v>
+        <v>45913.61797832176</v>
       </c>
       <c r="G134" s="2" t="n">
-        <v>45913.61797810689</v>
+        <v>45913.61797810185</v>
       </c>
       <c r="H134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr"/>
+      <c r="F135" s="2" t="n">
+        <v>45913.64054178241</v>
+      </c>
+      <c r="G135" s="2" t="n">
+        <v>45913.6405415625</v>
+      </c>
+      <c r="H135" t="inlineStr"/>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr"/>
+      <c r="F136" s="2" t="n">
+        <v>45913.64054178241</v>
+      </c>
+      <c r="G136" s="2" t="n">
+        <v>45913.6405415625</v>
+      </c>
+      <c r="H136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr"/>
+      <c r="F137" s="2" t="n">
+        <v>45913.64732755787</v>
+      </c>
+      <c r="G137" s="2" t="n">
+        <v>45913.6472990625</v>
+      </c>
+      <c r="H137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr"/>
+      <c r="F138" s="2" t="n">
+        <v>45913.65050219907</v>
+      </c>
+      <c r="G138" s="2" t="n">
+        <v>45913.65047331018</v>
+      </c>
+      <c r="H138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr"/>
+      <c r="F139" s="2" t="n">
+        <v>45913.65129641203</v>
+      </c>
+      <c r="G139" s="2" t="n">
+        <v>45913.65126802083</v>
+      </c>
+      <c r="H139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr"/>
+      <c r="F140" s="2" t="n">
+        <v>45913.65186983797</v>
+      </c>
+      <c r="G140" s="2" t="n">
+        <v>45913.65186961806</v>
+      </c>
+      <c r="H140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr"/>
+      <c r="F141" s="2" t="n">
+        <v>45913.65186983797</v>
+      </c>
+      <c r="G141" s="2" t="n">
+        <v>45913.65186961806</v>
+      </c>
+      <c r="H141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr"/>
+      <c r="F142" s="2" t="n">
+        <v>45913.65445490741</v>
+      </c>
+      <c r="G142" s="2" t="n">
+        <v>45913.65445467593</v>
+      </c>
+      <c r="H142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr"/>
+      <c r="F143" s="2" t="n">
+        <v>45913.65445490741</v>
+      </c>
+      <c r="G143" s="2" t="n">
+        <v>45913.65445467593</v>
+      </c>
+      <c r="H143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr"/>
+      <c r="F144" s="2" t="n">
+        <v>45913.6546618287</v>
+      </c>
+      <c r="G144" s="2" t="n">
+        <v>45913.65466160879</v>
+      </c>
+      <c r="H144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr"/>
+      <c r="F145" s="2" t="n">
+        <v>45913.6546618287</v>
+      </c>
+      <c r="G145" s="2" t="n">
+        <v>45913.65466160879</v>
+      </c>
+      <c r="H145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr"/>
+      <c r="F146" s="2" t="n">
+        <v>45913.65511253473</v>
+      </c>
+      <c r="G146" s="2" t="n">
+        <v>45913.65508446759</v>
+      </c>
+      <c r="H146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr"/>
+      <c r="F147" s="2" t="n">
+        <v>45913.65564542824</v>
+      </c>
+      <c r="G147" s="2" t="n">
+        <v>45913.65561700232</v>
+      </c>
+      <c r="H147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr"/>
+      <c r="F148" s="2" t="n">
+        <v>45913.66035568287</v>
+      </c>
+      <c r="G148" s="2" t="n">
+        <v>45913.66032637731</v>
+      </c>
+      <c r="H148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr"/>
+      <c r="F149" s="2" t="n">
+        <v>45913.66035568287</v>
+      </c>
+      <c r="G149" s="2" t="n">
+        <v>45913.66032637731</v>
+      </c>
+      <c r="H149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr"/>
+      <c r="F150" s="2" t="n">
+        <v>45913.66196864584</v>
+      </c>
+      <c r="G150" s="2" t="n">
+        <v>45913.6619391088</v>
+      </c>
+      <c r="H150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr"/>
+      <c r="F151" s="2" t="n">
+        <v>45913.66196864584</v>
+      </c>
+      <c r="G151" s="2" t="n">
+        <v>45913.6619391088</v>
+      </c>
+      <c r="H151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr"/>
+      <c r="F152" s="2" t="n">
+        <v>45913.67086850695</v>
+      </c>
+      <c r="G152" s="2" t="n">
+        <v>45913.67083818287</v>
+      </c>
+      <c r="H152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr"/>
+      <c r="F153" s="2" t="n">
+        <v>45913.67086850695</v>
+      </c>
+      <c r="G153" s="2" t="n">
+        <v>45913.67083818287</v>
+      </c>
+      <c r="H153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr"/>
+      <c r="F154" s="2" t="n">
+        <v>45913.67196922454</v>
+      </c>
+      <c r="G154" s="2" t="n">
+        <v>45913.67194067129</v>
+      </c>
+      <c r="H154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>(5)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr"/>
+      <c r="F155" s="2" t="n">
+        <v>45913.67196922454</v>
+      </c>
+      <c r="G155" s="2" t="n">
+        <v>45913.67194067129</v>
+      </c>
+      <c r="H155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>WeisfeilerLehman_SVC</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr"/>
+      <c r="F156" s="2" t="n">
+        <v>45913.72767268519</v>
+      </c>
+      <c r="G156" s="2" t="n">
+        <v>45913.7276703588</v>
+      </c>
+      <c r="H156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>WeisfeilerLehman_SVC</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr"/>
+      <c r="F157" s="2" t="n">
+        <v>45913.72767268519</v>
+      </c>
+      <c r="G157" s="2" t="n">
+        <v>45913.7276703588</v>
+      </c>
+      <c r="H157" t="inlineStr"/>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>VertexHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr"/>
+      <c r="F158" s="2" t="n">
+        <v>45913.72778729167</v>
+      </c>
+      <c r="G158" s="2" t="n">
+        <v>45913.72778664352</v>
+      </c>
+      <c r="H158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>VertexHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr"/>
+      <c r="F159" s="2" t="n">
+        <v>45913.72778729167</v>
+      </c>
+      <c r="G159" s="2" t="n">
+        <v>45913.72778664352</v>
+      </c>
+      <c r="H159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>EdgeHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr"/>
+      <c r="F160" s="2" t="n">
+        <v>45913.72780873843</v>
+      </c>
+      <c r="G160" s="2" t="n">
+        <v>45913.72780748842</v>
+      </c>
+      <c r="H160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>EdgeHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr"/>
+      <c r="F161" s="2" t="n">
+        <v>45913.72780873843</v>
+      </c>
+      <c r="G161" s="2" t="n">
+        <v>45913.72780748842</v>
+      </c>
+      <c r="H161" t="inlineStr"/>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>CombinedHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr"/>
+      <c r="F162" s="2" t="n">
+        <v>45913.72783034722</v>
+      </c>
+      <c r="G162" s="2" t="n">
+        <v>45913.72782857639</v>
+      </c>
+      <c r="H162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>CombinedHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr"/>
+      <c r="F163" s="2" t="n">
+        <v>45913.72783034722</v>
+      </c>
+      <c r="G163" s="2" t="n">
+        <v>45913.72782857639</v>
+      </c>
+      <c r="H163" t="inlineStr"/>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>NX_Histogram_SVC</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>SVC_NX_combined_Histogram_rbf</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>SVC_NX_combined_Histogram_rbf_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr"/>
+      <c r="F164" s="2" t="n">
+        <v>45913.72791674769</v>
+      </c>
+      <c r="G164" s="2" t="n">
+        <v>45913.72789449074</v>
+      </c>
+      <c r="H164" t="inlineStr"/>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>WeisfeilerLehman_SVC</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr"/>
+      <c r="F165" s="2" t="n">
+        <v>45913.73409707176</v>
+      </c>
+      <c r="G165" s="2" t="n">
+        <v>45913.73409509259</v>
+      </c>
+      <c r="H165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>WeisfeilerLehman_SVC</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr"/>
+      <c r="F166" s="2" t="n">
+        <v>45913.73409707176</v>
+      </c>
+      <c r="G166" s="2" t="n">
+        <v>45913.73409509259</v>
+      </c>
+      <c r="H166" t="inlineStr"/>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>VertexHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr"/>
+      <c r="F167" s="2" t="n">
+        <v>45913.73419482639</v>
+      </c>
+      <c r="G167" s="2" t="n">
+        <v>45913.73419340278</v>
+      </c>
+      <c r="H167" t="inlineStr"/>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>VertexHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr"/>
+      <c r="F168" s="2" t="n">
+        <v>45913.73419482639</v>
+      </c>
+      <c r="G168" s="2" t="n">
+        <v>45913.73419340278</v>
+      </c>
+      <c r="H168" t="inlineStr"/>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>EdgeHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr"/>
+      <c r="F169" s="2" t="n">
+        <v>45913.73421505787</v>
+      </c>
+      <c r="G169" s="2" t="n">
+        <v>45913.7342138426</v>
+      </c>
+      <c r="H169" t="inlineStr"/>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>EdgeHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr"/>
+      <c r="F170" s="2" t="n">
+        <v>45913.73421505787</v>
+      </c>
+      <c r="G170" s="2" t="n">
+        <v>45913.7342138426</v>
+      </c>
+      <c r="H170" t="inlineStr"/>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>CombinedHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr"/>
+      <c r="F171" s="2" t="n">
+        <v>45913.73423682871</v>
+      </c>
+      <c r="G171" s="2" t="n">
+        <v>45913.73423395833</v>
+      </c>
+      <c r="H171" t="inlineStr"/>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>CombinedHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr"/>
+      <c r="F172" s="2" t="n">
+        <v>45913.73423682871</v>
+      </c>
+      <c r="G172" s="2" t="n">
+        <v>45913.73423395833</v>
+      </c>
+      <c r="H172" t="inlineStr"/>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>NX_Histogram_SVC</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>SVC_NX_combined_Histogram_rbf</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>SVC_NX_combined_Histogram_rbf_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr"/>
+      <c r="F173" s="2" t="n">
+        <v>45913.7342797338</v>
+      </c>
+      <c r="G173" s="2" t="n">
+        <v>45913.73427939815</v>
+      </c>
+      <c r="H173" t="inlineStr"/>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>NX_Histogram_SVC</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>SVC_NX_combined_Histogram_rbf</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>SVC_NX_combined_Histogram_rbf_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr"/>
+      <c r="F174" s="2" t="n">
+        <v>45913.7342797338</v>
+      </c>
+      <c r="G174" s="2" t="n">
+        <v>45913.73427939815</v>
+      </c>
+      <c r="H174" t="inlineStr"/>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Blind_Classifier_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr"/>
+      <c r="F175" s="2" t="n">
+        <v>45913.73772368056</v>
+      </c>
+      <c r="G175" s="2" t="n">
+        <v>45913.73772363426</v>
+      </c>
+      <c r="H175" t="inlineStr"/>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Blind_Classifier_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr"/>
+      <c r="F176" s="2" t="n">
+        <v>45913.73772368056</v>
+      </c>
+      <c r="G176" s="2" t="n">
+        <v>45913.73772363426</v>
+      </c>
+      <c r="H176" t="inlineStr"/>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Random_Classifier</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr"/>
+      <c r="F177" s="2" t="n">
+        <v>45913.73772914352</v>
+      </c>
+      <c r="G177" s="2" t="n">
+        <v>45913.73772913194</v>
+      </c>
+      <c r="H177" t="inlineStr"/>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Random_Classifier</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr"/>
+      <c r="F178" s="2" t="n">
+        <v>45913.73772914352</v>
+      </c>
+      <c r="G178" s="2" t="n">
+        <v>45913.73772913194</v>
+      </c>
+      <c r="H178" t="inlineStr"/>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>GED_KNN</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr"/>
+      <c r="F179" s="2" t="n">
+        <v>45913.73773995371</v>
+      </c>
+      <c r="G179" s="2" t="n">
+        <v>45913.7377378588</v>
+      </c>
+      <c r="H179" t="inlineStr"/>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>GED_KNN</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr"/>
+      <c r="F180" s="2" t="n">
+        <v>45913.73773995371</v>
+      </c>
+      <c r="G180" s="2" t="n">
+        <v>45913.7377378588</v>
+      </c>
+      <c r="H180" t="inlineStr"/>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Base_GED_SVC</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr"/>
+      <c r="F181" s="2" t="n">
+        <v>45913.73805092592</v>
+      </c>
+      <c r="G181" s="2" t="n">
+        <v>45913.73804820602</v>
+      </c>
+      <c r="H181" t="inlineStr"/>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Base_GED_SVC</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr"/>
+      <c r="F182" s="2" t="n">
+        <v>45913.73805092592</v>
+      </c>
+      <c r="G182" s="2" t="n">
+        <v>45913.73804820602</v>
+      </c>
+      <c r="H182" t="inlineStr"/>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>WeisfeilerLehman_SVC</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr"/>
+      <c r="F183" s="2" t="n">
+        <v>45913.74150092593</v>
+      </c>
+      <c r="G183" s="2" t="n">
+        <v>45913.74149896991</v>
+      </c>
+      <c r="H183" t="inlineStr"/>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>VertexHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr"/>
+      <c r="F184" s="2" t="n">
+        <v>45913.74150371528</v>
+      </c>
+      <c r="G184" s="2" t="n">
+        <v>45913.74150259259</v>
+      </c>
+      <c r="H184" t="inlineStr"/>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>EdgeHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr"/>
+      <c r="F185" s="2" t="n">
+        <v>45913.7415065625</v>
+      </c>
+      <c r="G185" s="2" t="n">
+        <v>45913.7415050463</v>
+      </c>
+      <c r="H185" t="inlineStr"/>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>CombinedHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr"/>
+      <c r="F186" s="2" t="n">
+        <v>45913.74151126157</v>
+      </c>
+      <c r="G186" s="2" t="n">
+        <v>45913.74150787037</v>
+      </c>
+      <c r="H186" t="inlineStr"/>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>NX_Histogram_SVC</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>SVC_NX_combined_Histogram_rbf</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>SVC_NX_combined_Histogram_rbf_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr"/>
+      <c r="F187" s="2" t="n">
+        <v>45913.74151291667</v>
+      </c>
+      <c r="G187" s="2" t="n">
+        <v>45913.74151258102</v>
+      </c>
+      <c r="H187" t="inlineStr"/>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Blind_Classifier_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr"/>
+      <c r="F188" s="2" t="n">
+        <v>45913.74151423611</v>
+      </c>
+      <c r="G188" s="2" t="n">
+        <v>45913.74151418982</v>
+      </c>
+      <c r="H188" t="inlineStr"/>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Random_Classifier</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr"/>
+      <c r="F189" s="2" t="n">
+        <v>45913.74151543981</v>
+      </c>
+      <c r="G189" s="2" t="n">
+        <v>45913.74151542824</v>
+      </c>
+      <c r="H189" t="inlineStr"/>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>GED_KNN</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr"/>
+      <c r="F190" s="2" t="n">
+        <v>45913.74151877315</v>
+      </c>
+      <c r="G190" s="2" t="n">
+        <v>45913.74151664352</v>
+      </c>
+      <c r="H190" t="inlineStr"/>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Base_GED_SVC</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr"/>
+      <c r="F191" s="2" t="n">
+        <v>45913.7415230787</v>
+      </c>
+      <c r="G191" s="2" t="n">
+        <v>45913.74152054398</v>
+      </c>
+      <c r="H191" t="inlineStr"/>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_SVC_Base-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr"/>
+      <c r="F192" s="2" t="n">
+        <v>45913.75743936343</v>
+      </c>
+      <c r="G192" s="2" t="n">
+        <v>45913.75740873843</v>
+      </c>
+      <c r="H192" t="inlineStr"/>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>WeisfeilerLehman_SVC</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr"/>
+      <c r="F193" s="2" t="n">
+        <v>45913.75912180555</v>
+      </c>
+      <c r="G193" s="2" t="n">
+        <v>45913.75911980324</v>
+      </c>
+      <c r="H193" t="inlineStr"/>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>VertexHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr"/>
+      <c r="F194" s="2" t="n">
+        <v>45913.75912462963</v>
+      </c>
+      <c r="G194" s="2" t="n">
+        <v>45913.75912350694</v>
+      </c>
+      <c r="H194" t="inlineStr"/>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>EdgeHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr"/>
+      <c r="F195" s="2" t="n">
+        <v>45913.75912762732</v>
+      </c>
+      <c r="G195" s="2" t="n">
+        <v>45913.75912600695</v>
+      </c>
+      <c r="H195" t="inlineStr"/>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>CombinedHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr"/>
+      <c r="F196" s="2" t="n">
+        <v>45913.75913237269</v>
+      </c>
+      <c r="G196" s="2" t="n">
+        <v>45913.7591290162</v>
+      </c>
+      <c r="H196" t="inlineStr"/>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>NX_Histogram_SVC</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>SVC_NX_combined_Histogram_rbf</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>SVC_NX_combined_Histogram_rbf_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr"/>
+      <c r="F197" s="2" t="n">
+        <v>45913.75913407408</v>
+      </c>
+      <c r="G197" s="2" t="n">
+        <v>45913.75913373843</v>
+      </c>
+      <c r="H197" t="inlineStr"/>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Blind_Classifier_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr"/>
+      <c r="F198" s="2" t="n">
+        <v>45913.75913543982</v>
+      </c>
+      <c r="G198" s="2" t="n">
+        <v>45913.75913539352</v>
+      </c>
+      <c r="H198" t="inlineStr"/>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Random_Classifier</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr"/>
+      <c r="F199" s="2" t="n">
+        <v>45913.75913670139</v>
+      </c>
+      <c r="G199" s="2" t="n">
+        <v>45913.75913668981</v>
+      </c>
+      <c r="H199" t="inlineStr"/>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>GED_KNN</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr"/>
+      <c r="F200" s="2" t="n">
+        <v>45913.75914</v>
+      </c>
+      <c r="G200" s="2" t="n">
+        <v>45913.75913793981</v>
+      </c>
+      <c r="H200" t="inlineStr"/>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Base_GED_SVC</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr"/>
+      <c r="F201" s="2" t="n">
+        <v>45913.7591447801</v>
+      </c>
+      <c r="G201" s="2" t="n">
+        <v>45913.75914224537</v>
+      </c>
+      <c r="H201" t="inlineStr"/>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>DIFFUSION_GED_SVC</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr"/>
+      <c r="F202" s="2" t="n">
+        <v>45913.75914881944</v>
+      </c>
+      <c r="G202" s="2" t="n">
+        <v>45913.75914665509</v>
+      </c>
+      <c r="H202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Trivial_GED_SVC</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>SVC_Trivial-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>SVC_Trivial-GED_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr"/>
+      <c r="F203" s="2" t="n">
+        <v>45913.75915319444</v>
+      </c>
+      <c r="G203" s="2" t="n">
+        <v>45913.75915061343</v>
+      </c>
+      <c r="H203" t="inlineStr"/>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Simple_Prototype_GED_SVC</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>SVC_Simple_Prototype_GED_poly</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>SVC_Simple_Prototype_GED_poly_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr"/>
+      <c r="F204" s="2" t="n">
+        <v>45913.7591571412</v>
+      </c>
+      <c r="G204" s="2" t="n">
+        <v>45913.75915510417</v>
+      </c>
+      <c r="H204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>ZERO_GED_SVC</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr"/>
+      <c r="F205" s="2" t="n">
+        <v>45913.75919875</v>
+      </c>
+      <c r="G205" s="2" t="n">
+        <v>45913.7591584375</v>
+      </c>
+      <c r="H205" t="inlineStr"/>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>WeisfeilerLehman_SVC</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr"/>
+      <c r="F206" s="2" t="n">
+        <v>45913.76580666667</v>
+      </c>
+      <c r="G206" s="2" t="n">
+        <v>45913.76580467592</v>
+      </c>
+      <c r="H206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>WeisfeilerLehman_SVC</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr"/>
+      <c r="F207" s="2" t="n">
+        <v>45913.76580666667</v>
+      </c>
+      <c r="G207" s="2" t="n">
+        <v>45913.76580467592</v>
+      </c>
+      <c r="H207" t="inlineStr"/>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>VertexHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr"/>
+      <c r="F208" s="2" t="n">
+        <v>45913.765909375</v>
+      </c>
+      <c r="G208" s="2" t="n">
+        <v>45913.765908125</v>
+      </c>
+      <c r="H208" t="inlineStr"/>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>VertexHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr"/>
+      <c r="F209" s="2" t="n">
+        <v>45913.765909375</v>
+      </c>
+      <c r="G209" s="2" t="n">
+        <v>45913.765908125</v>
+      </c>
+      <c r="H209" t="inlineStr"/>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>EdgeHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr"/>
+      <c r="F210" s="2" t="n">
+        <v>45913.76593446759</v>
+      </c>
+      <c r="G210" s="2" t="n">
+        <v>45913.76593327546</v>
+      </c>
+      <c r="H210" t="inlineStr"/>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>EdgeHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr"/>
+      <c r="F211" s="2" t="n">
+        <v>45913.76593446759</v>
+      </c>
+      <c r="G211" s="2" t="n">
+        <v>45913.76593327546</v>
+      </c>
+      <c r="H211" t="inlineStr"/>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>CombinedHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr"/>
+      <c r="F212" s="2" t="n">
+        <v>45913.76595641204</v>
+      </c>
+      <c r="G212" s="2" t="n">
+        <v>45913.76595368056</v>
+      </c>
+      <c r="H212" t="inlineStr"/>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>CombinedHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr"/>
+      <c r="F213" s="2" t="n">
+        <v>45913.76595641204</v>
+      </c>
+      <c r="G213" s="2" t="n">
+        <v>45913.76595368056</v>
+      </c>
+      <c r="H213" t="inlineStr"/>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>Blind_Classifier_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr"/>
+      <c r="F214" s="2" t="n">
+        <v>45913.76600538194</v>
+      </c>
+      <c r="G214" s="2" t="n">
+        <v>45913.76600534722</v>
+      </c>
+      <c r="H214" t="inlineStr"/>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Blind_Classifier_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr"/>
+      <c r="F215" s="2" t="n">
+        <v>45913.76600538194</v>
+      </c>
+      <c r="G215" s="2" t="n">
+        <v>45913.76600534722</v>
+      </c>
+      <c r="H215" t="inlineStr"/>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>Random_Classifier</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr"/>
+      <c r="F216" s="2" t="n">
+        <v>45913.76601087963</v>
+      </c>
+      <c r="G216" s="2" t="n">
+        <v>45913.76601086806</v>
+      </c>
+      <c r="H216" t="inlineStr"/>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>Random_Classifier</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr"/>
+      <c r="F217" s="2" t="n">
+        <v>45913.76601087963</v>
+      </c>
+      <c r="G217" s="2" t="n">
+        <v>45913.76601086806</v>
+      </c>
+      <c r="H217" t="inlineStr"/>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>GED_KNN</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>ENZYMES</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED_trained_on_ENZYMES.joblib</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr"/>
+      <c r="F218" s="2" t="n">
+        <v>45913.76602247686</v>
+      </c>
+      <c r="G218" s="2" t="n">
+        <v>45913.7660203125</v>
+      </c>
+      <c r="H218" t="inlineStr"/>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>WeisfeilerLehman_SVC</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr"/>
+      <c r="F219" s="2" t="n">
+        <v>45913.77742121528</v>
+      </c>
+      <c r="G219" s="2" t="n">
+        <v>45913.77742072917</v>
+      </c>
+      <c r="H219" t="inlineStr"/>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>WeisfeilerLehman_SVC</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr"/>
+      <c r="F220" s="2" t="n">
+        <v>45913.77742121528</v>
+      </c>
+      <c r="G220" s="2" t="n">
+        <v>45913.77742072917</v>
+      </c>
+      <c r="H220" t="inlineStr"/>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>VertexHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr"/>
+      <c r="F221" s="2" t="n">
+        <v>45913.7774569213</v>
+      </c>
+      <c r="G221" s="2" t="n">
+        <v>45913.77745672454</v>
+      </c>
+      <c r="H221" t="inlineStr"/>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>VertexHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr"/>
+      <c r="F222" s="2" t="n">
+        <v>45913.7774569213</v>
+      </c>
+      <c r="G222" s="2" t="n">
+        <v>45913.77745672454</v>
+      </c>
+      <c r="H222" t="inlineStr"/>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>EdgeHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr"/>
+      <c r="F223" s="2" t="n">
+        <v>45913.77746459491</v>
+      </c>
+      <c r="G223" s="2" t="n">
+        <v>45913.77746444444</v>
+      </c>
+      <c r="H223" t="inlineStr"/>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>EdgeHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr"/>
+      <c r="F224" s="2" t="n">
+        <v>45913.77746459491</v>
+      </c>
+      <c r="G224" s="2" t="n">
+        <v>45913.77746444444</v>
+      </c>
+      <c r="H224" t="inlineStr"/>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>CombinedHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr"/>
+      <c r="F225" s="2" t="n">
+        <v>45913.77747375</v>
+      </c>
+      <c r="G225" s="2" t="n">
+        <v>45913.77747347222</v>
+      </c>
+      <c r="H225" t="inlineStr"/>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>CombinedHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr"/>
+      <c r="F226" s="2" t="n">
+        <v>45913.77747375</v>
+      </c>
+      <c r="G226" s="2" t="n">
+        <v>45913.77747347222</v>
+      </c>
+      <c r="H226" t="inlineStr"/>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Blind_Classifier_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr"/>
+      <c r="F227" s="2" t="n">
+        <v>45913.77748542824</v>
+      </c>
+      <c r="G227" s="2" t="n">
+        <v>45913.77748541666</v>
+      </c>
+      <c r="H227" t="inlineStr"/>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Blind_Classifier_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr"/>
+      <c r="F228" s="2" t="n">
+        <v>45913.77748542824</v>
+      </c>
+      <c r="G228" s="2" t="n">
+        <v>45913.77748541666</v>
+      </c>
+      <c r="H228" t="inlineStr"/>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Random_Classifier</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr"/>
+      <c r="F229" s="2" t="n">
+        <v>45913.77748913194</v>
+      </c>
+      <c r="G229" s="2" t="n">
+        <v>45913.77748912037</v>
+      </c>
+      <c r="H229" t="inlineStr"/>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Random_Classifier</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr"/>
+      <c r="F230" s="2" t="n">
+        <v>45913.77748913194</v>
+      </c>
+      <c r="G230" s="2" t="n">
+        <v>45913.77748912037</v>
+      </c>
+      <c r="H230" t="inlineStr"/>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>GED_KNN</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr"/>
+      <c r="F231" s="2" t="n">
+        <v>45913.77749597222</v>
+      </c>
+      <c r="G231" s="2" t="n">
+        <v>45913.7774952662</v>
+      </c>
+      <c r="H231" t="inlineStr"/>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>WeisfeilerLehman_SVC</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr"/>
+      <c r="F232" s="2" t="n">
+        <v>45913.77913434028</v>
+      </c>
+      <c r="G232" s="2" t="n">
+        <v>45913.77913383102</v>
+      </c>
+      <c r="H232" t="inlineStr"/>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>WeisfeilerLehman_SVC</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>SVC_WeisfeilerLehman_5_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr"/>
+      <c r="F233" s="2" t="n">
+        <v>45913.77913434028</v>
+      </c>
+      <c r="G233" s="2" t="n">
+        <v>45913.77913383102</v>
+      </c>
+      <c r="H233" t="inlineStr"/>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>VertexHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr"/>
+      <c r="F234" s="2" t="n">
+        <v>45913.77916840278</v>
+      </c>
+      <c r="G234" s="2" t="n">
+        <v>45913.7791682176</v>
+      </c>
+      <c r="H234" t="inlineStr"/>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>VertexHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr"/>
+      <c r="F235" s="2" t="n">
+        <v>45913.77916840278</v>
+      </c>
+      <c r="G235" s="2" t="n">
+        <v>45913.7791682176</v>
+      </c>
+      <c r="H235" t="inlineStr"/>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>EdgeHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr"/>
+      <c r="F236" s="2" t="n">
+        <v>45913.77917584491</v>
+      </c>
+      <c r="G236" s="2" t="n">
+        <v>45913.77917570602</v>
+      </c>
+      <c r="H236" t="inlineStr"/>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>EdgeHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr"/>
+      <c r="F237" s="2" t="n">
+        <v>45913.77917584491</v>
+      </c>
+      <c r="G237" s="2" t="n">
+        <v>45913.77917570602</v>
+      </c>
+      <c r="H237" t="inlineStr"/>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>CombinedHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr"/>
+      <c r="F238" s="2" t="n">
+        <v>45913.77918513889</v>
+      </c>
+      <c r="G238" s="2" t="n">
+        <v>45913.77918490741</v>
+      </c>
+      <c r="H238" t="inlineStr"/>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>CombinedHistogram_SVC</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr"/>
+      <c r="F239" s="2" t="n">
+        <v>45913.77918513889</v>
+      </c>
+      <c r="G239" s="2" t="n">
+        <v>45913.77918490741</v>
+      </c>
+      <c r="H239" t="inlineStr"/>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>Blind_Classifier_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr"/>
+      <c r="F240" s="2" t="n">
+        <v>45913.77919666667</v>
+      </c>
+      <c r="G240" s="2" t="n">
+        <v>45913.77919665509</v>
+      </c>
+      <c r="H240" t="inlineStr"/>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>Blind_Classifier</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>Blind_Classifier_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr"/>
+      <c r="F241" s="2" t="n">
+        <v>45913.77919666667</v>
+      </c>
+      <c r="G241" s="2" t="n">
+        <v>45913.77919665509</v>
+      </c>
+      <c r="H241" t="inlineStr"/>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Random_Classifier</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr"/>
+      <c r="F242" s="2" t="n">
+        <v>45913.7792002662</v>
+      </c>
+      <c r="G242" s="2" t="n">
+        <v>45913.77920025463</v>
+      </c>
+      <c r="H242" t="inlineStr"/>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Random_Classifier</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>RandomGuesser_uniform_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr"/>
+      <c r="F243" s="2" t="n">
+        <v>45913.7792002662</v>
+      </c>
+      <c r="G243" s="2" t="n">
+        <v>45913.77920025463</v>
+      </c>
+      <c r="H243" t="inlineStr"/>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>GED_KNN</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr"/>
+      <c r="F244" s="2" t="n">
+        <v>45913.7792075</v>
+      </c>
+      <c r="G244" s="2" t="n">
+        <v>45913.77920675926</v>
+      </c>
+      <c r="H244" t="inlineStr"/>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>GED_KNN</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>(1)-NN_Classifier_GED_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr"/>
+      <c r="F245" s="2" t="n">
+        <v>45913.7792075</v>
+      </c>
+      <c r="G245" s="2" t="n">
+        <v>45913.77920675926</v>
+      </c>
+      <c r="H245" t="inlineStr"/>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Base_GED_SVC</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr"/>
+      <c r="F246" s="2" t="n">
+        <v>45913.7803690625</v>
+      </c>
+      <c r="G246" s="2" t="n">
+        <v>45913.78036820602</v>
+      </c>
+      <c r="H246" t="inlineStr"/>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Base_GED_SVC</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>SVC_Base-GED_precomputed_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr"/>
+      <c r="F247" s="2" t="n">
+        <v>45913.78036906252</v>
+      </c>
+      <c r="G247" s="2" t="n">
+        <v>45913.7803682099</v>
+      </c>
+      <c r="H247" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
i copied all the GEd-classifiers and i feixed the Prototype Selection
</commit_message>
<xml_diff>
--- a/configs/test_diagnostics.xlsx
+++ b/configs/test_diagnostics.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H374"/>
+  <dimension ref="A1:H403"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11176,12 +11176,882 @@
       </c>
       <c r="E374" t="inlineStr"/>
       <c r="F374" s="2" t="n">
-        <v>45915.67773759227</v>
+        <v>45915.6777375926</v>
       </c>
       <c r="G374" s="2" t="n">
-        <v>45915.6777373615</v>
+        <v>45915.67773736111</v>
       </c>
       <c r="H374" t="inlineStr"/>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E375" t="inlineStr"/>
+      <c r="F375" s="2" t="n">
+        <v>45915.90239358796</v>
+      </c>
+      <c r="G375" s="2" t="n">
+        <v>45915.90238939815</v>
+      </c>
+      <c r="H375" t="inlineStr"/>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr"/>
+      <c r="F376" s="2" t="n">
+        <v>45915.90305</v>
+      </c>
+      <c r="G376" s="2" t="n">
+        <v>45915.90283905093</v>
+      </c>
+      <c r="H376" t="inlineStr"/>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E377" t="inlineStr"/>
+      <c r="F377" s="2" t="n">
+        <v>45915.91021627315</v>
+      </c>
+      <c r="G377" s="2" t="n">
+        <v>45915.90968631944</v>
+      </c>
+      <c r="H377" t="inlineStr"/>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr"/>
+      <c r="F378" s="2" t="n">
+        <v>45915.91075240741</v>
+      </c>
+      <c r="G378" s="2" t="n">
+        <v>45915.91060165509</v>
+      </c>
+      <c r="H378" t="inlineStr"/>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E379" t="inlineStr"/>
+      <c r="F379" s="2" t="n">
+        <v>45915.91097590278</v>
+      </c>
+      <c r="G379" s="2" t="n">
+        <v>45915.91097273148</v>
+      </c>
+      <c r="H379" t="inlineStr"/>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr"/>
+      <c r="F380" s="2" t="n">
+        <v>45915.92173537037</v>
+      </c>
+      <c r="G380" s="2" t="n">
+        <v>45915.92173221065</v>
+      </c>
+      <c r="H380" t="inlineStr"/>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr"/>
+      <c r="F381" s="2" t="n">
+        <v>45915.9218982176</v>
+      </c>
+      <c r="G381" s="2" t="n">
+        <v>45915.92189467593</v>
+      </c>
+      <c r="H381" t="inlineStr"/>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr"/>
+      <c r="F382" s="2" t="n">
+        <v>45915.92199268519</v>
+      </c>
+      <c r="G382" s="2" t="n">
+        <v>45915.92198901621</v>
+      </c>
+      <c r="H382" t="inlineStr"/>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr"/>
+      <c r="F383" s="2" t="n">
+        <v>45915.92215949074</v>
+      </c>
+      <c r="G383" s="2" t="n">
+        <v>45915.92215592592</v>
+      </c>
+      <c r="H383" t="inlineStr"/>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr"/>
+      <c r="F384" s="2" t="n">
+        <v>45915.92252958333</v>
+      </c>
+      <c r="G384" s="2" t="n">
+        <v>45915.92252607639</v>
+      </c>
+      <c r="H384" t="inlineStr"/>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E385" t="inlineStr"/>
+      <c r="F385" s="2" t="n">
+        <v>45915.92266288195</v>
+      </c>
+      <c r="G385" s="2" t="n">
+        <v>45915.92265982639</v>
+      </c>
+      <c r="H385" t="inlineStr"/>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E386" t="inlineStr"/>
+      <c r="F386" s="2" t="n">
+        <v>45915.92331371528</v>
+      </c>
+      <c r="G386" s="2" t="n">
+        <v>45915.92331065972</v>
+      </c>
+      <c r="H386" t="inlineStr"/>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E387" t="inlineStr"/>
+      <c r="F387" s="2" t="n">
+        <v>45915.92477596065</v>
+      </c>
+      <c r="G387" s="2" t="n">
+        <v>45915.92477296296</v>
+      </c>
+      <c r="H387" t="inlineStr"/>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E388" t="inlineStr"/>
+      <c r="F388" s="2" t="n">
+        <v>45915.92644039352</v>
+      </c>
+      <c r="G388" s="2" t="n">
+        <v>45915.92643734954</v>
+      </c>
+      <c r="H388" t="inlineStr"/>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E389" t="inlineStr"/>
+      <c r="F389" s="2" t="n">
+        <v>45915.92711929399</v>
+      </c>
+      <c r="G389" s="2" t="n">
+        <v>45915.92711626158</v>
+      </c>
+      <c r="H389" t="inlineStr"/>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E390" t="inlineStr"/>
+      <c r="F390" s="2" t="n">
+        <v>45915.92757193287</v>
+      </c>
+      <c r="G390" s="2" t="n">
+        <v>45915.92756888889</v>
+      </c>
+      <c r="H390" t="inlineStr"/>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E391" t="inlineStr"/>
+      <c r="F391" s="2" t="n">
+        <v>45915.92806930556</v>
+      </c>
+      <c r="G391" s="2" t="n">
+        <v>45915.92806621527</v>
+      </c>
+      <c r="H391" t="inlineStr"/>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E392" t="inlineStr"/>
+      <c r="F392" s="2" t="n">
+        <v>45915.93155193287</v>
+      </c>
+      <c r="G392" s="2" t="n">
+        <v>45915.93094765046</v>
+      </c>
+      <c r="H392" t="inlineStr"/>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E393" t="inlineStr"/>
+      <c r="F393" s="2" t="n">
+        <v>45915.95589414352</v>
+      </c>
+      <c r="G393" s="2" t="n">
+        <v>45915.9558908912</v>
+      </c>
+      <c r="H393" t="inlineStr"/>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E394" t="inlineStr"/>
+      <c r="F394" s="2" t="n">
+        <v>45915.9568825</v>
+      </c>
+      <c r="G394" s="2" t="n">
+        <v>45915.95687934028</v>
+      </c>
+      <c r="H394" t="inlineStr"/>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E395" t="inlineStr"/>
+      <c r="F395" s="2" t="n">
+        <v>45915.95900917824</v>
+      </c>
+      <c r="G395" s="2" t="n">
+        <v>45915.95900587963</v>
+      </c>
+      <c r="H395" t="inlineStr"/>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr"/>
+      <c r="F396" s="2" t="n">
+        <v>45915.96002582176</v>
+      </c>
+      <c r="G396" s="2" t="n">
+        <v>45915.96002253472</v>
+      </c>
+      <c r="H396" t="inlineStr"/>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr"/>
+      <c r="F397" s="2" t="n">
+        <v>45915.96197258102</v>
+      </c>
+      <c r="G397" s="2" t="n">
+        <v>45915.96196956019</v>
+      </c>
+      <c r="H397" t="inlineStr"/>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_linear_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr"/>
+      <c r="F398" s="2" t="n">
+        <v>45915.96344083334</v>
+      </c>
+      <c r="G398" s="2" t="n">
+        <v>45915.96343762732</v>
+      </c>
+      <c r="H398" t="inlineStr"/>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr"/>
+      <c r="F399" s="2" t="n">
+        <v>45915.97400869213</v>
+      </c>
+      <c r="G399" s="2" t="n">
+        <v>45915.97400861111</v>
+      </c>
+      <c r="H399" t="inlineStr"/>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E400" t="inlineStr"/>
+      <c r="F400" s="2" t="n">
+        <v>45915.97696756945</v>
+      </c>
+      <c r="G400" s="2" t="n">
+        <v>45915.97696747685</v>
+      </c>
+      <c r="H400" t="inlineStr"/>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E401" t="inlineStr"/>
+      <c r="F401" s="2" t="n">
+        <v>45915.97728130787</v>
+      </c>
+      <c r="G401" s="2" t="n">
+        <v>45915.97723453704</v>
+      </c>
+      <c r="H401" t="inlineStr"/>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E402" t="inlineStr"/>
+      <c r="F402" s="2" t="n">
+        <v>45915.97757503473</v>
+      </c>
+      <c r="G402" s="2" t="n">
+        <v>45915.97757493056</v>
+      </c>
+      <c r="H402" t="inlineStr"/>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E403" t="inlineStr"/>
+      <c r="F403" s="2" t="n">
+        <v>45915.97782832831</v>
+      </c>
+      <c r="G403" s="2" t="n">
+        <v>45915.97782822531</v>
+      </c>
+      <c r="H403" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed AUC and got results speed up the Zero Kernel
</commit_message>
<xml_diff>
--- a/configs/test_diagnostics.xlsx
+++ b/configs/test_diagnostics.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H487"/>
+  <dimension ref="A1:H527"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14566,12 +14566,1212 @@
       </c>
       <c r="E487" t="inlineStr"/>
       <c r="F487" s="2" t="n">
-        <v>45924.50271661561</v>
+        <v>45924.50271662037</v>
       </c>
       <c r="G487" s="2" t="n">
-        <v>45924.50266360275</v>
+        <v>45924.50266359954</v>
       </c>
       <c r="H487" t="inlineStr"/>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E488" t="inlineStr"/>
+      <c r="F488" s="2" t="n">
+        <v>45924.62051621528</v>
+      </c>
+      <c r="G488" s="2" t="n">
+        <v>45924.6204903125</v>
+      </c>
+      <c r="H488" t="inlineStr"/>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E489" t="inlineStr"/>
+      <c r="F489" s="2" t="n">
+        <v>45924.65678487268</v>
+      </c>
+      <c r="G489" s="2" t="n">
+        <v>45924.65678231481</v>
+      </c>
+      <c r="H489" t="inlineStr"/>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E490" t="inlineStr"/>
+      <c r="F490" s="2" t="n">
+        <v>45924.6660155787</v>
+      </c>
+      <c r="G490" s="2" t="n">
+        <v>45924.66601310185</v>
+      </c>
+      <c r="H490" t="inlineStr"/>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E491" t="inlineStr"/>
+      <c r="F491" s="2" t="n">
+        <v>45924.6660155787</v>
+      </c>
+      <c r="G491" s="2" t="n">
+        <v>45924.66601310185</v>
+      </c>
+      <c r="H491" t="inlineStr"/>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E492" t="inlineStr"/>
+      <c r="F492" s="2" t="n">
+        <v>45924.66860956018</v>
+      </c>
+      <c r="G492" s="2" t="n">
+        <v>45924.66860641204</v>
+      </c>
+      <c r="H492" t="inlineStr"/>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E493" t="inlineStr"/>
+      <c r="F493" s="2" t="n">
+        <v>45924.66860956018</v>
+      </c>
+      <c r="G493" s="2" t="n">
+        <v>45924.66860641204</v>
+      </c>
+      <c r="H493" t="inlineStr"/>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E494" t="inlineStr"/>
+      <c r="F494" s="2" t="n">
+        <v>45924.67399969907</v>
+      </c>
+      <c r="G494" s="2" t="n">
+        <v>45924.67399782407</v>
+      </c>
+      <c r="H494" t="inlineStr"/>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E495" t="inlineStr"/>
+      <c r="F495" s="2" t="n">
+        <v>45924.67574260417</v>
+      </c>
+      <c r="G495" s="2" t="n">
+        <v>45924.67574130787</v>
+      </c>
+      <c r="H495" t="inlineStr"/>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E496" t="inlineStr"/>
+      <c r="F496" s="2" t="n">
+        <v>45924.67574260417</v>
+      </c>
+      <c r="G496" s="2" t="n">
+        <v>45924.67574130787</v>
+      </c>
+      <c r="H496" t="inlineStr"/>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E497" t="inlineStr"/>
+      <c r="F497" s="2" t="n">
+        <v>45924.67655055555</v>
+      </c>
+      <c r="G497" s="2" t="n">
+        <v>45924.67654515046</v>
+      </c>
+      <c r="H497" t="inlineStr"/>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E498" t="inlineStr"/>
+      <c r="F498" s="2" t="n">
+        <v>45924.68070023148</v>
+      </c>
+      <c r="G498" s="2" t="n">
+        <v>45924.68069513889</v>
+      </c>
+      <c r="H498" t="inlineStr"/>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E499" t="inlineStr"/>
+      <c r="F499" s="2" t="n">
+        <v>45925.51793018518</v>
+      </c>
+      <c r="G499" s="2" t="n">
+        <v>45925.51783008102</v>
+      </c>
+      <c r="H499" t="inlineStr"/>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D500" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E500" t="inlineStr"/>
+      <c r="F500" s="2" t="n">
+        <v>45925.52300373842</v>
+      </c>
+      <c r="G500" s="2" t="n">
+        <v>45925.52189148148</v>
+      </c>
+      <c r="H500" t="inlineStr"/>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E501" t="inlineStr"/>
+      <c r="F501" s="2" t="n">
+        <v>45925.52649340278</v>
+      </c>
+      <c r="G501" s="2" t="n">
+        <v>45925.52648737268</v>
+      </c>
+      <c r="H501" t="inlineStr"/>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E502" t="inlineStr"/>
+      <c r="F502" s="2" t="n">
+        <v>45925.53015548611</v>
+      </c>
+      <c r="G502" s="2" t="n">
+        <v>45925.53014549769</v>
+      </c>
+      <c r="H502" t="inlineStr"/>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E503" t="inlineStr"/>
+      <c r="F503" s="2" t="n">
+        <v>45925.54304729166</v>
+      </c>
+      <c r="G503" s="2" t="n">
+        <v>45925.54304013889</v>
+      </c>
+      <c r="H503" t="inlineStr"/>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E504" t="inlineStr"/>
+      <c r="F504" s="2" t="n">
+        <v>45925.54304729166</v>
+      </c>
+      <c r="G504" s="2" t="n">
+        <v>45925.54304013889</v>
+      </c>
+      <c r="H504" t="inlineStr"/>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E505" t="inlineStr"/>
+      <c r="F505" s="2" t="n">
+        <v>45925.54536806713</v>
+      </c>
+      <c r="G505" s="2" t="n">
+        <v>45925.54536305556</v>
+      </c>
+      <c r="H505" t="inlineStr"/>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E506" t="inlineStr"/>
+      <c r="F506" s="2" t="n">
+        <v>45925.54850828704</v>
+      </c>
+      <c r="G506" s="2" t="n">
+        <v>45925.54850324074</v>
+      </c>
+      <c r="H506" t="inlineStr"/>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E507" t="inlineStr"/>
+      <c r="F507" s="2" t="n">
+        <v>45925.55185165509</v>
+      </c>
+      <c r="G507" s="2" t="n">
+        <v>45925.55184623843</v>
+      </c>
+      <c r="H507" t="inlineStr"/>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E508" t="inlineStr"/>
+      <c r="F508" s="2" t="n">
+        <v>45925.55185165509</v>
+      </c>
+      <c r="G508" s="2" t="n">
+        <v>45925.55184623843</v>
+      </c>
+      <c r="H508" t="inlineStr"/>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E509" t="inlineStr"/>
+      <c r="F509" s="2" t="n">
+        <v>45925.57046309028</v>
+      </c>
+      <c r="G509" s="2" t="n">
+        <v>45925.57028105324</v>
+      </c>
+      <c r="H509" t="inlineStr"/>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E510" t="inlineStr"/>
+      <c r="F510" s="2" t="n">
+        <v>45925.57171554398</v>
+      </c>
+      <c r="G510" s="2" t="n">
+        <v>45925.57147372685</v>
+      </c>
+      <c r="H510" t="inlineStr"/>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E511" t="inlineStr"/>
+      <c r="F511" s="2" t="n">
+        <v>45925.57743530093</v>
+      </c>
+      <c r="G511" s="2" t="n">
+        <v>45925.57673060185</v>
+      </c>
+      <c r="H511" t="inlineStr"/>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="D512" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E512" t="inlineStr"/>
+      <c r="F512" s="2" t="n">
+        <v>45925.58201896991</v>
+      </c>
+      <c r="G512" s="2" t="n">
+        <v>45925.58174378472</v>
+      </c>
+      <c r="H512" t="inlineStr"/>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E513" t="inlineStr"/>
+      <c r="F513" s="2" t="n">
+        <v>45925.58601043982</v>
+      </c>
+      <c r="G513" s="2" t="n">
+        <v>45925.58583722222</v>
+      </c>
+      <c r="H513" t="inlineStr"/>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E514" t="inlineStr"/>
+      <c r="F514" s="2" t="n">
+        <v>45925.58601043982</v>
+      </c>
+      <c r="G514" s="2" t="n">
+        <v>45925.58583722222</v>
+      </c>
+      <c r="H514" t="inlineStr"/>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(7)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>(7)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D515" t="inlineStr">
+        <is>
+          <t>(7)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E515" t="inlineStr"/>
+      <c r="F515" s="2" t="n">
+        <v>45926.55947094908</v>
+      </c>
+      <c r="G515" s="2" t="n">
+        <v>45926.55942363426</v>
+      </c>
+      <c r="H515" t="inlineStr"/>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_(7)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>(7)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D516" t="inlineStr">
+        <is>
+          <t>(7)-NN_Classifier_GED_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E516" t="inlineStr"/>
+      <c r="F516" s="2" t="n">
+        <v>45926.56548694445</v>
+      </c>
+      <c r="G516" s="2" t="n">
+        <v>45926.56548652778</v>
+      </c>
+      <c r="H516" t="inlineStr"/>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D517" t="inlineStr">
+        <is>
+          <t>SVC_Simple-Prototype-GED_poly_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E517" t="inlineStr"/>
+      <c r="F517" s="2" t="n">
+        <v>45926.56598181713</v>
+      </c>
+      <c r="G517" s="2" t="n">
+        <v>45926.56597805556</v>
+      </c>
+      <c r="H517" t="inlineStr"/>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_Letter-high_with_(7)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Letter-high</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>(7)-NN_Classifier_GED</t>
+        </is>
+      </c>
+      <c r="D518" t="inlineStr">
+        <is>
+          <t>(7)-NN_Classifier_GED_trained_on_Letter-high.joblib</t>
+        </is>
+      </c>
+      <c r="E518" t="inlineStr"/>
+      <c r="F518" s="2" t="n">
+        <v>45926.57018256944</v>
+      </c>
+      <c r="G518" s="2" t="n">
+        <v>45926.57013594908</v>
+      </c>
+      <c r="H518" t="inlineStr"/>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D519" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E519" t="inlineStr"/>
+      <c r="F519" s="2" t="n">
+        <v>45926.60692478009</v>
+      </c>
+      <c r="G519" s="2" t="n">
+        <v>45926.60692107639</v>
+      </c>
+      <c r="H519" t="inlineStr"/>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D520" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E520" t="inlineStr"/>
+      <c r="F520" s="2" t="n">
+        <v>45926.60778174768</v>
+      </c>
+      <c r="G520" s="2" t="n">
+        <v>45926.60777612268</v>
+      </c>
+      <c r="H520" t="inlineStr"/>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D521" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E521" t="inlineStr"/>
+      <c r="F521" s="2" t="n">
+        <v>45926.60778174768</v>
+      </c>
+      <c r="G521" s="2" t="n">
+        <v>45926.60777612268</v>
+      </c>
+      <c r="H521" t="inlineStr"/>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D522" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E522" t="inlineStr"/>
+      <c r="F522" s="2" t="n">
+        <v>45926.63602863426</v>
+      </c>
+      <c r="G522" s="2" t="n">
+        <v>45926.63602075232</v>
+      </c>
+      <c r="H522" t="inlineStr"/>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D523" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E523" t="inlineStr"/>
+      <c r="F523" s="2" t="n">
+        <v>45926.6371171412</v>
+      </c>
+      <c r="G523" s="2" t="n">
+        <v>45926.63710895833</v>
+      </c>
+      <c r="H523" t="inlineStr"/>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E524" t="inlineStr"/>
+      <c r="F524" s="2" t="n">
+        <v>45926.65641547454</v>
+      </c>
+      <c r="G524" s="2" t="n">
+        <v>45926.65641295139</v>
+      </c>
+      <c r="H524" t="inlineStr"/>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E525" t="inlineStr"/>
+      <c r="F525" s="2" t="n">
+        <v>45926.66002355324</v>
+      </c>
+      <c r="G525" s="2" t="n">
+        <v>45926.66002107639</v>
+      </c>
+      <c r="H525" t="inlineStr"/>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_BZR_with_SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>BZR</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>SVC_Zero-GED_precomputed_trained_on_BZR.joblib</t>
+        </is>
+      </c>
+      <c r="E526" t="inlineStr"/>
+      <c r="F526" s="2" t="n">
+        <v>45926.66002355324</v>
+      </c>
+      <c r="G526" s="2" t="n">
+        <v>45926.66002107639</v>
+      </c>
+      <c r="H526" t="inlineStr"/>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Trivial-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>SVC_Trivial-GED_precomputed</t>
+        </is>
+      </c>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>SVC_Trivial-GED_precomputed_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E527" t="inlineStr"/>
+      <c r="F527" s="2" t="n">
+        <v>45926.82500684206</v>
+      </c>
+      <c r="G527" s="2" t="n">
+        <v>45926.82500614467</v>
+      </c>
+      <c r="H527" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added Attributed data, and broke things
</commit_message>
<xml_diff>
--- a/configs/test_diagnostics.xlsx
+++ b/configs/test_diagnostics.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H574"/>
+  <dimension ref="A1:H596"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17176,12 +17176,672 @@
       </c>
       <c r="E574" t="inlineStr"/>
       <c r="F574" s="2" t="n">
-        <v>45929.47446090107</v>
+        <v>45929.47446090278</v>
       </c>
       <c r="G574" s="2" t="n">
-        <v>45929.47446027765</v>
+        <v>45929.47446027778</v>
       </c>
       <c r="H574" t="inlineStr"/>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_feature-KNN</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>feature-KNN</t>
+        </is>
+      </c>
+      <c r="D575" t="inlineStr">
+        <is>
+          <t>feature-KNN_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E575" t="inlineStr"/>
+      <c r="F575" s="2" t="n">
+        <v>45934.69965002315</v>
+      </c>
+      <c r="G575" s="2" t="n">
+        <v>45934.6996496875</v>
+      </c>
+      <c r="H575" t="inlineStr"/>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Hybrid-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>SVC_Hybrid-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D576" t="inlineStr">
+        <is>
+          <t>SVC_Hybrid-Prototype-GED_poly_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E576" t="inlineStr"/>
+      <c r="F576" s="2" t="n">
+        <v>45934.73216295139</v>
+      </c>
+      <c r="G576" s="2" t="n">
+        <v>45934.73216259259</v>
+      </c>
+      <c r="H576" t="inlineStr"/>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_PTC_FR_with_SVC_Hybrid-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>PTC_FR</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>SVC_Hybrid-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D577" t="inlineStr">
+        <is>
+          <t>SVC_Hybrid-Prototype-GED_poly_trained_on_PTC_FR.joblib</t>
+        </is>
+      </c>
+      <c r="E577" t="inlineStr"/>
+      <c r="F577" s="2" t="n">
+        <v>45934.74649184028</v>
+      </c>
+      <c r="G577" s="2" t="n">
+        <v>45934.74649076389</v>
+      </c>
+      <c r="H577" t="inlineStr"/>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_VertexHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="D578" t="inlineStr">
+        <is>
+          <t>SVC_VertexHistogram_rbf_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E578" t="inlineStr"/>
+      <c r="F578" s="2" t="n">
+        <v>45934.77812075231</v>
+      </c>
+      <c r="G578" s="2" t="n">
+        <v>45934.77806451389</v>
+      </c>
+      <c r="H578" t="inlineStr"/>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_EdgeHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="D579" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_rbf_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E579" t="inlineStr"/>
+      <c r="F579" s="2" t="n">
+        <v>45934.78180104167</v>
+      </c>
+      <c r="G579" s="2" t="n">
+        <v>45934.78180091435</v>
+      </c>
+      <c r="H579" t="inlineStr"/>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_EdgeHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="D580" t="inlineStr">
+        <is>
+          <t>SVC_EdgeHistogram_rbf_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E580" t="inlineStr"/>
+      <c r="F580" s="2" t="n">
+        <v>45934.78180104167</v>
+      </c>
+      <c r="G580" s="2" t="n">
+        <v>45934.78180091435</v>
+      </c>
+      <c r="H580" t="inlineStr"/>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_CombinedHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="D581" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_rbf_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E581" t="inlineStr"/>
+      <c r="F581" s="2" t="n">
+        <v>45934.84572197917</v>
+      </c>
+      <c r="G581" s="2" t="n">
+        <v>45934.8457218287</v>
+      </c>
+      <c r="H581" t="inlineStr"/>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_CombinedHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="D582" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_rbf_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E582" t="inlineStr"/>
+      <c r="F582" s="2" t="n">
+        <v>45934.84572197917</v>
+      </c>
+      <c r="G582" s="2" t="n">
+        <v>45934.8457218287</v>
+      </c>
+      <c r="H582" t="inlineStr"/>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_CombinedHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="D583" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_rbf_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E583" t="inlineStr"/>
+      <c r="F583" s="2" t="n">
+        <v>45934.85872717592</v>
+      </c>
+      <c r="G583" s="2" t="n">
+        <v>45934.85872704861</v>
+      </c>
+      <c r="H583" t="inlineStr"/>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_CombinedHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="D584" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_rbf_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E584" t="inlineStr"/>
+      <c r="F584" s="2" t="n">
+        <v>45934.85872717592</v>
+      </c>
+      <c r="G584" s="2" t="n">
+        <v>45934.85872704861</v>
+      </c>
+      <c r="H584" t="inlineStr"/>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_CombinedHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_rbf</t>
+        </is>
+      </c>
+      <c r="D585" t="inlineStr">
+        <is>
+          <t>SVC_CombinedHistogram_rbf_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E585" t="inlineStr"/>
+      <c r="F585" s="2" t="n">
+        <v>45934.86840295139</v>
+      </c>
+      <c r="G585" s="2" t="n">
+        <v>45934.86824746527</v>
+      </c>
+      <c r="H585" t="inlineStr"/>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_feature-KNN</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>feature-KNN</t>
+        </is>
+      </c>
+      <c r="D586" t="inlineStr">
+        <is>
+          <t>feature-KNN_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E586" t="inlineStr"/>
+      <c r="F586" s="2" t="n">
+        <v>45934.87197950231</v>
+      </c>
+      <c r="G586" s="2" t="n">
+        <v>45934.87197908565</v>
+      </c>
+      <c r="H586" t="inlineStr"/>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_feature-KNN</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>feature-KNN</t>
+        </is>
+      </c>
+      <c r="D587" t="inlineStr">
+        <is>
+          <t>feature-KNN_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E587" t="inlineStr"/>
+      <c r="F587" s="2" t="n">
+        <v>45934.87640118055</v>
+      </c>
+      <c r="G587" s="2" t="n">
+        <v>45934.87640077547</v>
+      </c>
+      <c r="H587" t="inlineStr"/>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_feature-KNN</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>feature-KNN</t>
+        </is>
+      </c>
+      <c r="D588" t="inlineStr">
+        <is>
+          <t>feature-KNN_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E588" t="inlineStr"/>
+      <c r="F588" s="2" t="n">
+        <v>45934.88721842592</v>
+      </c>
+      <c r="G588" s="2" t="n">
+        <v>45934.88689296296</v>
+      </c>
+      <c r="H588" t="inlineStr"/>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_feature-KNN</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>feature-KNN</t>
+        </is>
+      </c>
+      <c r="D589" t="inlineStr">
+        <is>
+          <t>feature-KNN_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E589" t="inlineStr"/>
+      <c r="F589" s="2" t="n">
+        <v>45934.88872850694</v>
+      </c>
+      <c r="G589" s="2" t="n">
+        <v>45934.88872775463</v>
+      </c>
+      <c r="H589" t="inlineStr"/>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Hybrid-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>SVC_Hybrid-Prototype-GED_poly</t>
+        </is>
+      </c>
+      <c r="D590" t="inlineStr">
+        <is>
+          <t>SVC_Hybrid-Prototype-GED_poly_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E590" t="inlineStr"/>
+      <c r="F590" s="2" t="n">
+        <v>45934.98598952546</v>
+      </c>
+      <c r="G590" s="2" t="n">
+        <v>45934.98598822916</v>
+      </c>
+      <c r="H590" t="inlineStr"/>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="D591" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E591" t="inlineStr"/>
+      <c r="F591" s="2" t="n">
+        <v>45935.12126365741</v>
+      </c>
+      <c r="G591" s="2" t="n">
+        <v>45935.12125907408</v>
+      </c>
+      <c r="H591" t="inlineStr"/>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="D592" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E592" t="inlineStr"/>
+      <c r="F592" s="2" t="n">
+        <v>45935.12517533565</v>
+      </c>
+      <c r="G592" s="2" t="n">
+        <v>45935.12517086806</v>
+      </c>
+      <c r="H592" t="inlineStr"/>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="D593" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E593" t="inlineStr"/>
+      <c r="F593" s="2" t="n">
+        <v>45935.12592638889</v>
+      </c>
+      <c r="G593" s="2" t="n">
+        <v>45935.12592527777</v>
+      </c>
+      <c r="H593" t="inlineStr"/>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="D594" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E594" t="inlineStr"/>
+      <c r="F594" s="2" t="n">
+        <v>45935.12736097222</v>
+      </c>
+      <c r="G594" s="2" t="n">
+        <v>45935.12736019676</v>
+      </c>
+      <c r="H594" t="inlineStr"/>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="D595" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E595" t="inlineStr"/>
+      <c r="F595" s="2" t="n">
+        <v>45935.70941407407</v>
+      </c>
+      <c r="G595" s="2" t="n">
+        <v>45935.70941309028</v>
+      </c>
+      <c r="H595" t="inlineStr"/>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>Fucntionality_test_MUTAG_with_SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>MUTAG</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed</t>
+        </is>
+      </c>
+      <c r="D596" t="inlineStr">
+        <is>
+          <t>SVC_Random-Walk-Edit_precomputed_trained_on_MUTAG.joblib</t>
+        </is>
+      </c>
+      <c r="E596" t="inlineStr"/>
+      <c r="F596" s="2" t="n">
+        <v>45935.70991768294</v>
+      </c>
+      <c r="G596" s="2" t="n">
+        <v>45935.70991684647</v>
+      </c>
+      <c r="H596" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>